<commit_message>
ci: add third form
</commit_message>
<xml_diff>
--- a/ONCHO/Breeding Site Survey/Cote d'Ivoire/civ_oncho_bsa_1_river_assessment_202208.xlsx
+++ b/ONCHO/Breeding Site Survey/Cote d'Ivoire/civ_oncho_bsa_1_river_assessment_202208.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="192">
   <si>
     <t>type</t>
   </si>
@@ -91,7 +91,7 @@
     <t>s_region</t>
   </si>
   <si>
-    <t>Sélectionner un département</t>
+    <t>Sélectionner une région sanitaire</t>
   </si>
   <si>
     <t>zone_transmission = ${s_zone_transmission}</t>
@@ -124,9 +124,6 @@
     <t>Sélectionner un site</t>
   </si>
   <si>
-    <t>district = ${s_district}</t>
-  </si>
-  <si>
     <t>s_river_basin_name</t>
   </si>
   <si>
@@ -160,7 +157,7 @@
     <t>s_tidc_date</t>
   </si>
   <si>
-    <t>Date de lancement du TIDC</t>
+    <t>Date de début de traitement</t>
   </si>
   <si>
     <t>Exemple : Août 2022</t>
@@ -193,7 +190,7 @@
     <t>s_close_village</t>
   </si>
   <si>
-    <t xml:space="preserve">Village sous traitement TIDC le plus proche </t>
+    <t xml:space="preserve">Village le plus proche </t>
   </si>
   <si>
     <t>s_close_village_population</t>
@@ -553,10 +550,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Juillet 2022) 1. Enquête Entomologique d'ONCHO - Inspection de la rivière V3</t>
-  </si>
-  <si>
-    <t>civ_oncho_bsa_1_river_assessment_202208</t>
+    <t>(Août 2022) 1. Enquête Entomologique d'ONCHO - Inspection de la rivière V2</t>
+  </si>
+  <si>
+    <t>civ_oncho_bsa_1_river_assessment_202208_v2</t>
   </si>
   <si>
     <t>French</t>
@@ -603,10 +600,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -700,46 +697,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -754,10 +713,39 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -776,6 +764,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -785,22 +780,23 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -822,22 +818,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -900,13 +897,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -918,31 +957,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -954,19 +969,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -978,13 +993,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1002,37 +1029,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1044,43 +1065,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1172,17 +1169,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1192,6 +1189,24 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1222,15 +1237,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1246,178 +1252,169 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="35" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1478,9 +1475,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1929,11 +1923,11 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1953,109 +1947,109 @@
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="1" ht="18" spans="1:13">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="61"/>
+      <c r="M1" s="60"/>
     </row>
     <row r="2" s="4" customFormat="1" ht="28.5" spans="1:11">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="48" t="s">
+      <c r="E2" s="39"/>
+      <c r="F2" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40" t="s">
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="40"/>
+      <c r="K2" s="39"/>
     </row>
     <row r="3" s="4" customFormat="1" spans="1:11">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
     </row>
     <row r="4" s="4" customFormat="1" ht="28.5" spans="1:12">
       <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="58" t="s">
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="52" t="s">
+      <c r="L4" s="51" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2063,22 +2057,22 @@
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="54" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="58" t="s">
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="54" t="s">
+      <c r="L5" s="53" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2086,14 +2080,14 @@
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="J6" s="58" t="s">
+      <c r="D6" s="53"/>
+      <c r="J6" s="57" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2101,129 +2095,127 @@
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="J7" s="58" t="s">
+      <c r="D7" s="53"/>
+      <c r="J7" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="54" t="s">
+      <c r="L7" s="53"/>
+    </row>
+    <row r="8" s="4" customFormat="1" spans="1:12">
+      <c r="A8" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="39" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" s="4" customFormat="1" spans="1:12">
-      <c r="A8" s="50" t="s">
+      <c r="C8" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+    </row>
+    <row r="9" s="4" customFormat="1" spans="1:12">
+      <c r="A9" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="51" t="s">
+      <c r="B9" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40" t="s">
+      <c r="C9" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-    </row>
-    <row r="9" s="4" customFormat="1" spans="1:12">
-      <c r="A9" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="51" t="s">
+      <c r="K9" s="39"/>
+      <c r="L9" s="47"/>
+    </row>
+    <row r="10" s="4" customFormat="1" ht="28.5" spans="1:12">
+      <c r="A10" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40" t="s">
+      <c r="C10" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="50"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="40"/>
-      <c r="L9" s="48"/>
-    </row>
-    <row r="10" s="4" customFormat="1" ht="28.5" spans="1:12">
-      <c r="A10" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="48"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="47"/>
     </row>
     <row r="11" s="4" customFormat="1" spans="1:10">
       <c r="A11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="C11" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="54"/>
-      <c r="J11" s="58" t="s">
+      <c r="D11" s="53"/>
+      <c r="J11" s="57" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>47</v>
       </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="58" t="s">
+      <c r="J12" s="57" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="58" t="s">
+      <c r="J13" s="57" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2232,26 +2224,26 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
         <v>52</v>
       </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" s="58" t="s">
+      <c r="J14" s="57" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
         <v>54</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>55</v>
       </c>
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J15" s="58" t="s">
+      <c r="J15" s="57" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2260,151 +2252,151 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
         <v>57</v>
       </c>
-      <c r="C16" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" s="58"/>
+      <c r="J16" s="57"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="J17" s="58"/>
+      <c r="J17" s="57"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>62</v>
       </c>
-      <c r="C18" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" s="58"/>
+      <c r="J18" s="57"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
         <v>64</v>
       </c>
-      <c r="C19" t="s">
+      <c r="H19" t="s">
         <v>65</v>
       </c>
-      <c r="H19" t="s">
-        <v>66</v>
-      </c>
-      <c r="J19" s="58"/>
+      <c r="J19" s="57"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
         <v>67</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>68</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>69</v>
       </c>
-      <c r="D20" t="s">
+      <c r="J20" s="57" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" s="4" customFormat="1" spans="1:12">
+      <c r="A21" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="J20" s="58" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" s="4" customFormat="1" spans="1:12">
-      <c r="A21" s="50" t="s">
+      <c r="B21" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="56" t="s">
+      <c r="C21" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="57" t="s">
+      <c r="D21" s="56"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+    </row>
+    <row r="22" s="4" customFormat="1" ht="28.5" spans="1:12">
+      <c r="A22" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="57"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-    </row>
-    <row r="22" s="4" customFormat="1" ht="28.5" spans="1:12">
-      <c r="A22" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="56" t="s">
+      <c r="C22" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="57" t="s">
+      <c r="D22" s="56"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="H22" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="57"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="H22" t="s">
+      <c r="I22" s="49"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+    </row>
+    <row r="23" s="4" customFormat="1" spans="1:12">
+      <c r="A23" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="I22" s="50"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="50"/>
-    </row>
-    <row r="23" s="4" customFormat="1" spans="1:12">
-      <c r="A23" s="50" t="s">
+      <c r="B23" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+    </row>
+    <row r="24" s="4" customFormat="1" spans="1:12">
+      <c r="A24" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-    </row>
-    <row r="24" s="4" customFormat="1" spans="1:12">
-      <c r="A24" s="50" t="s">
+      <c r="B24" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="50"/>
-      <c r="L24" s="50"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
     </row>
     <row r="25" s="4" customFormat="1" spans="2:7">
-      <c r="B25" s="54"/>
-      <c r="D25" s="54"/>
+      <c r="B25" s="53"/>
+      <c r="D25" s="53"/>
       <c r="G25"/>
     </row>
     <row r="26" s="4" customFormat="1" spans="2:7">
-      <c r="B26" s="54"/>
-      <c r="D26" s="54"/>
+      <c r="B26" s="53"/>
+      <c r="D26" s="53"/>
       <c r="G26"/>
     </row>
     <row r="27" s="4" customFormat="1" spans="2:7">
@@ -2440,573 +2432,573 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="F1" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="37" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="39" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="40" t="s">
+      <c r="B2" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="C2" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="D2" s="41"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="40"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="41"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="41" t="s">
+      <c r="C3" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="D3" s="41"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="40"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="41"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="41" t="s">
+      <c r="C4" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="D4" s="41"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="40"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="41"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="43" t="s">
+      <c r="B5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="62" t="s">
+      <c r="C7" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="D7" s="43"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="44"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="62" t="s">
+      <c r="C8" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8" s="44"/>
+      <c r="D8" s="43"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="C11" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="C13" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="45" t="s">
-        <v>110</v>
+      <c r="C15" s="44" t="s">
+        <v>109</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B16" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" s="45" t="s">
-        <v>111</v>
+        <v>108</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>110</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="45" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>111</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>113</v>
+        <v>108</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>112</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="45" t="s">
         <v>114</v>
-      </c>
-      <c r="C19" s="46" t="s">
-        <v>115</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B20" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="45" t="s">
         <v>116</v>
-      </c>
-      <c r="C20" s="46" t="s">
-        <v>117</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>119</v>
+      <c r="C21" s="45" t="s">
+        <v>118</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B22" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>119</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B23" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23" s="46" t="s">
-        <v>121</v>
+        <v>117</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>120</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="45" t="s">
         <v>122</v>
-      </c>
-      <c r="C24" s="46" t="s">
-        <v>123</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B25" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="45" t="s">
         <v>124</v>
-      </c>
-      <c r="C25" s="46" t="s">
-        <v>125</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="C26" s="44" t="s">
         <v>127</v>
-      </c>
-      <c r="C26" s="45" t="s">
-        <v>128</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="44" t="s">
         <v>129</v>
-      </c>
-      <c r="C27" s="45" t="s">
-        <v>130</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="44" t="s">
         <v>131</v>
-      </c>
-      <c r="C28" s="45" t="s">
-        <v>132</v>
       </c>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="44" t="s">
         <v>133</v>
-      </c>
-      <c r="C29" s="45" t="s">
-        <v>134</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B30" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="44" t="s">
         <v>135</v>
-      </c>
-      <c r="C30" s="45" t="s">
-        <v>136</v>
       </c>
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="46" t="s">
         <v>137</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>138</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B32" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="44" t="s">
         <v>139</v>
-      </c>
-      <c r="C32" s="45" t="s">
-        <v>140</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B33" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="44" t="s">
         <v>141</v>
-      </c>
-      <c r="C33" s="45" t="s">
-        <v>142</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B34" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="44" t="s">
         <v>124</v>
-      </c>
-      <c r="C34" s="45" t="s">
-        <v>125</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -3016,317 +3008,317 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="2:4">
@@ -3350,7 +3342,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -3360,25 +3352,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>176</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" t="s">
         <v>178</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>179</v>
-      </c>
-      <c r="C2" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -3414,84 +3406,84 @@
   <sheetData>
     <row r="1" ht="63.75" spans="1:20">
       <c r="A1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" ht="23.25" spans="1:20">
       <c r="A2" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="21" t="s">
-        <v>191</v>
+      <c r="G2" s="10" t="s">
+        <v>190</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
+        <v>153</v>
+      </c>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
       <c r="S2" s="18"/>
       <c r="T2" s="7"/>
     </row>
     <row r="3" ht="23.25" spans="1:20">
       <c r="A3" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="22"/>
-      <c r="G3" s="23" t="s">
-        <v>192</v>
+      <c r="E3" s="21"/>
+      <c r="G3" s="22" t="s">
+        <v>191</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -3500,22 +3492,22 @@
     </row>
     <row r="4" ht="23.25" spans="1:20">
       <c r="A4" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="22"/>
+      <c r="E4" s="21"/>
       <c r="G4" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
@@ -3524,103 +3516,103 @@
     </row>
     <row r="5" ht="23.25" spans="1:20">
       <c r="A5" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="20"/>
       <c r="N5" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="31"/>
+        <v>156</v>
+      </c>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="30"/>
       <c r="S5" s="9"/>
       <c r="T5" s="11"/>
     </row>
     <row r="6" ht="23.25" spans="1:20">
       <c r="A6" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="6"/>
       <c r="E6" s="20"/>
       <c r="N6" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="32"/>
-      <c r="S6" s="33"/>
+        <v>157</v>
+      </c>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="31"/>
+      <c r="S6" s="32"/>
       <c r="T6" s="7"/>
     </row>
     <row r="7" ht="23.25" spans="1:20">
       <c r="A7" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="22"/>
+      <c r="E7" s="21"/>
       <c r="N7" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="P7" s="29"/>
+        <v>158</v>
+      </c>
+      <c r="P7" s="28"/>
       <c r="Q7" s="9"/>
-      <c r="S7" s="33"/>
+      <c r="S7" s="32"/>
       <c r="T7" s="6"/>
     </row>
     <row r="8" ht="23.25" spans="1:20">
       <c r="A8" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="22"/>
+      <c r="E8" s="21"/>
       <c r="N8" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
-      <c r="S8" s="33"/>
+      <c r="S8" s="32"/>
       <c r="T8" s="6"/>
     </row>
     <row r="9" ht="23.25" spans="1:20">
       <c r="A9" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="22"/>
+      <c r="E9" s="21"/>
       <c r="N9" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="12"/>
@@ -3629,19 +3621,19 @@
     </row>
     <row r="10" ht="23.25" spans="1:20">
       <c r="A10" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="6"/>
       <c r="E10" s="20"/>
       <c r="N10" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="12"/>
@@ -3650,19 +3642,19 @@
     </row>
     <row r="11" ht="21" spans="1:20">
       <c r="A11" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="24"/>
+      <c r="E11" s="23"/>
       <c r="N11" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="13"/>
@@ -3671,19 +3663,19 @@
     </row>
     <row r="12" ht="23.25" spans="1:20">
       <c r="A12" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="22"/>
+      <c r="E12" s="21"/>
       <c r="N12" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="13"/>
@@ -3692,19 +3684,19 @@
     </row>
     <row r="13" ht="23.25" spans="1:20">
       <c r="A13" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="N13" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="14"/>
@@ -3713,200 +3705,200 @@
     </row>
     <row r="14" ht="23.25" spans="1:20">
       <c r="A14" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="22"/>
+      <c r="E14" s="21"/>
       <c r="N14" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P14" s="5"/>
       <c r="Q14" s="18"/>
-      <c r="S14" s="34"/>
+      <c r="S14" s="33"/>
       <c r="T14" s="7"/>
     </row>
     <row r="15" ht="23.25" spans="1:20">
       <c r="A15" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="6"/>
       <c r="E15" s="20"/>
       <c r="N15" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P15" s="5"/>
-      <c r="Q15" s="35"/>
+      <c r="Q15" s="34"/>
       <c r="S15" s="9"/>
       <c r="T15" s="7"/>
     </row>
     <row r="16" ht="23.25" spans="1:20">
       <c r="A16" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="6"/>
       <c r="E16" s="20"/>
       <c r="N16" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P16" s="5"/>
-      <c r="Q16" s="35"/>
+      <c r="Q16" s="34"/>
       <c r="S16" s="9"/>
       <c r="T16" s="6"/>
     </row>
     <row r="17" ht="23.25" spans="1:20">
       <c r="A17" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="6"/>
       <c r="E17" s="20"/>
       <c r="N17" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
-      <c r="S17" s="35"/>
+      <c r="S17" s="34"/>
       <c r="T17" s="15"/>
     </row>
     <row r="18" ht="23.25" spans="1:20">
       <c r="A18" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="6"/>
       <c r="E18" s="20"/>
       <c r="N18" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P18" s="9"/>
-      <c r="Q18" s="33"/>
+      <c r="Q18" s="32"/>
       <c r="S18" s="12"/>
       <c r="T18" s="7"/>
     </row>
     <row r="19" ht="23.25" spans="1:20">
       <c r="A19" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="22"/>
+      <c r="E19" s="21"/>
       <c r="N19" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P19" s="9"/>
-      <c r="Q19" s="27"/>
+      <c r="Q19" s="26"/>
       <c r="S19" s="12"/>
       <c r="T19" s="7"/>
     </row>
     <row r="20" ht="23.25" spans="1:20">
       <c r="A20" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="6"/>
       <c r="E20" s="20"/>
       <c r="N20" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="P20" s="30"/>
+        <v>171</v>
+      </c>
+      <c r="P20" s="29"/>
       <c r="Q20" s="16"/>
       <c r="S20" s="12"/>
       <c r="T20" s="7"/>
     </row>
     <row r="21" ht="23.25" spans="1:20">
       <c r="A21" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="11"/>
-      <c r="E21" s="22"/>
+      <c r="E21" s="21"/>
       <c r="N21" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="19"/>
-      <c r="S21" s="27"/>
+      <c r="S21" s="26"/>
       <c r="T21" s="7"/>
     </row>
     <row r="22" ht="23.25" spans="1:20">
       <c r="A22" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="11"/>
-      <c r="E22" s="22"/>
+      <c r="E22" s="21"/>
       <c r="N22" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="13"/>
-      <c r="S22" s="35"/>
+      <c r="S22" s="34"/>
       <c r="T22" s="6"/>
     </row>
     <row r="23" ht="23.25" spans="1:20">
       <c r="A23" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="22"/>
+      <c r="E23" s="21"/>
       <c r="S23" s="5"/>
       <c r="T23" s="7"/>
     </row>
     <row r="24" ht="23.25" spans="1:20">
       <c r="A24" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="6"/>
@@ -3916,20 +3908,20 @@
     </row>
     <row r="25" ht="23.25" spans="1:20">
       <c r="A25" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="22"/>
-      <c r="S25" s="35"/>
+      <c r="E25" s="21"/>
+      <c r="S25" s="34"/>
       <c r="T25" s="17"/>
     </row>
     <row r="26" ht="23.25" spans="1:20">
       <c r="A26" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="13"/>
@@ -3940,40 +3932,40 @@
     </row>
     <row r="27" ht="23.25" spans="1:20">
       <c r="A27" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="13"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="22"/>
+      <c r="E27" s="21"/>
       <c r="S27" s="9"/>
       <c r="T27" s="7"/>
     </row>
     <row r="28" ht="23.25" spans="1:20">
       <c r="A28" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="13"/>
       <c r="D28" s="6"/>
       <c r="E28" s="20"/>
-      <c r="S28" s="27"/>
+      <c r="S28" s="26"/>
       <c r="T28" s="7"/>
     </row>
     <row r="29" ht="23.25" spans="1:20">
       <c r="A29" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="13"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="22"/>
+      <c r="E29" s="21"/>
       <c r="S29" s="13"/>
       <c r="T29" s="6"/>
     </row>
     <row r="30" ht="23.25" spans="1:20">
       <c r="A30" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="13"/>
@@ -3984,29 +3976,29 @@
     </row>
     <row r="31" ht="21" spans="1:20">
       <c r="A31" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="14"/>
       <c r="D31" s="15"/>
-      <c r="E31" s="25"/>
+      <c r="E31" s="24"/>
       <c r="S31" s="13"/>
       <c r="T31" s="6"/>
     </row>
     <row r="32" ht="21" spans="1:20">
       <c r="A32" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="14"/>
       <c r="D32" s="15"/>
-      <c r="E32" s="25"/>
+      <c r="E32" s="24"/>
       <c r="S32" s="13"/>
       <c r="T32" s="6"/>
     </row>
     <row r="33" ht="23.25" spans="1:20">
       <c r="A33" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="12"/>
@@ -4017,7 +4009,7 @@
     </row>
     <row r="34" ht="23.25" spans="1:20">
       <c r="A34" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="12"/>
@@ -4028,7 +4020,7 @@
     </row>
     <row r="35" ht="23.25" spans="1:20">
       <c r="A35" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="12"/>
@@ -4039,73 +4031,73 @@
     </row>
     <row r="36" ht="23.25" spans="1:20">
       <c r="A36" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="16"/>
       <c r="D36" s="17"/>
-      <c r="E36" s="26"/>
-      <c r="S36" s="33"/>
+      <c r="E36" s="25"/>
+      <c r="S36" s="32"/>
       <c r="T36" s="7"/>
     </row>
     <row r="37" ht="23.25" spans="1:20">
       <c r="A37" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="16"/>
       <c r="D37" s="6"/>
       <c r="E37" s="20"/>
-      <c r="S37" s="33"/>
+      <c r="S37" s="32"/>
       <c r="T37" s="6"/>
     </row>
     <row r="38" ht="23.25" spans="1:20">
       <c r="A38" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="18"/>
       <c r="D38" s="7"/>
-      <c r="E38" s="22"/>
+      <c r="E38" s="21"/>
       <c r="S38" s="9"/>
       <c r="T38" s="6"/>
     </row>
     <row r="39" ht="23.25" spans="1:20">
       <c r="A39" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="18"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="22"/>
+      <c r="E39" s="21"/>
       <c r="S39" s="9"/>
       <c r="T39" s="6"/>
     </row>
     <row r="40" ht="23.25" spans="1:20">
       <c r="A40" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="16"/>
       <c r="D40" s="15"/>
       <c r="E40" s="20"/>
-      <c r="S40" s="33"/>
+      <c r="S40" s="32"/>
       <c r="T40" s="6"/>
     </row>
     <row r="41" ht="23.25" spans="1:20">
       <c r="A41" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="19"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="22"/>
+      <c r="E41" s="21"/>
       <c r="S41" s="7"/>
       <c r="T41" s="6"/>
     </row>
     <row r="42" ht="23.25" spans="1:20">
       <c r="A42" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="13"/>
@@ -4116,12 +4108,12 @@
     </row>
     <row r="43" ht="23.25" spans="1:20">
       <c r="A43" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="13"/>
       <c r="D43" s="7"/>
-      <c r="E43" s="22"/>
+      <c r="E43" s="21"/>
       <c r="S43" s="13"/>
       <c r="T43" s="6"/>
     </row>

</xml_diff>